<commit_message>
Agregadas imagenes, agregado cambio en notebook main para que se vaya entendiendo - Falta agregar mas texto
</commit_message>
<xml_diff>
--- a/Others/Models.xlsx
+++ b/Others/Models.xlsx
@@ -1,27 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AB9F5D-9122-47F3-B82D-FC3B3041740E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804A03B4-9320-4EEC-8DB5-A8202A34DA90}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Paramétros" sheetId="2" r:id="rId1"/>
     <sheet name="Modelos" sheetId="1" r:id="rId2"/>
+    <sheet name="Algoritmos Clásicos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Accuracy - Train</t>
   </si>
@@ -129,6 +135,27 @@
   </si>
   <si>
     <t>Validation Dataset Size</t>
+  </si>
+  <si>
+    <t>Algoritmo</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>Ada Boost Classifier</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Se utilizaron 200 iteraciones para realizar el entrenamiento</t>
+  </si>
+  <si>
+    <t>Se utilizaron 100 iteraciones para realizar el entrenamiento</t>
   </si>
 </sst>
 </file>
@@ -156,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +199,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -203,7 +236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,6 +261,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis2" xfId="1" builtinId="33"/>
@@ -292,6 +326,18 @@
     <tableColumn id="7" xr3:uid="{C8FE7198-9B64-4A7D-9280-F57BDF3819EA}" name="Epochs"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94B26180-966B-402B-9F3D-9913811FDE4D}" name="Tabla2" displayName="Tabla2" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4" xr:uid="{C0E4A5E8-7DEC-4CD3-B373-AD11DAE6FC5B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B71C4E9F-D39F-4DCD-BF42-A6B94DA86295}" name="Algoritmo"/>
+    <tableColumn id="2" xr3:uid="{4554B2CE-290B-4051-9BE0-F9D06CF2ECD4}" name="Accuracy"/>
+    <tableColumn id="3" xr3:uid="{6E2BCFE8-A57F-4326-ACC6-30074AF543B1}" name="Otros"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -558,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2663BD0-1F66-4864-81E0-3FA8E24E1B3D}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,45 +617,59 @@
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="5">
         <v>20000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="5">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="5">
         <v>128</v>
       </c>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E4" s="3">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -617,14 +677,16 @@
         <f>E5*(1-E4)</f>
         <v>2880000</v>
       </c>
+      <c r="C5" s="10"/>
       <c r="D5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="6">
         <v>3600000</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -632,14 +694,22 @@
         <f>E5*E4</f>
         <v>720000</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="5">
         <v>400000</v>
       </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -653,14 +723,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
@@ -1052,7 +1122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1078,7 +1148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1142,7 +1212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1156,7 +1226,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1170,7 +1240,7 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1189,4 +1259,68 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693943A1-8369-4B18-A67E-7A453A65E1FA}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>0.43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>0.49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>0.51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>